<commit_message>
Revisão e atualização do codigo
</commit_message>
<xml_diff>
--- a/tabela_energia_solar.xlsx
+++ b/tabela_energia_solar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,17 +436,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Media Geracao Anual</t>
+          <t>Mês</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Eficiencia media</t>
+          <t>Geração Mensal (kWh)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Meses com Producao Abaixo do Esperado</t>
+          <t>Eficiência Média Mensal</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -456,189 +456,920 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Media Anual abaixo</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Economia Anual</t>
+          <t>Economia Mensal</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>16128.38</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>jan/23</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>0.795</v>
+        <v>14018.03507989479</v>
       </c>
       <c r="C2" t="n">
+        <v>0.9235312949144248</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>fev/23</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>14949.49595783571</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9246679758811538</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>mar/23</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>14537.74260832353</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8824736461578573</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>abr/23</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>18279.91016327494</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.8613172748742098</v>
+      </c>
+      <c r="D5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" t="n">
+        <v>11250</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>mai/23</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>16255.19719269662</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.8502538146157599</v>
+      </c>
+      <c r="D6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>jun/23</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>13805.29103056303</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.8168052326229519</v>
+      </c>
+      <c r="D7" t="n">
+        <v>11</v>
+      </c>
+      <c r="E7" t="n">
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>jul/23</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>13941.99561851709</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.7929034671484142</v>
+      </c>
+      <c r="D8" t="n">
+        <v>11</v>
+      </c>
+      <c r="E8" t="n">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>ago/23</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>15474.86621416792</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.7756964490890278</v>
+      </c>
+      <c r="D9" t="n">
+        <v>12</v>
+      </c>
+      <c r="E9" t="n">
+        <v>26250</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>set/23</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>14726.45210408088</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.7787962977969178</v>
+      </c>
+      <c r="D10" t="n">
+        <v>14</v>
+      </c>
+      <c r="E10" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>out/23</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>15528.80960014159</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.7810320899749387</v>
+      </c>
+      <c r="D11" t="n">
+        <v>14</v>
+      </c>
+      <c r="E11" t="n">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>nov/23</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>15414.1665471413</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.7827224030655975</v>
+      </c>
+      <c r="D12" t="n">
+        <v>17</v>
+      </c>
+      <c r="E12" t="n">
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>dez/23</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>20772.72079654977</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.7947069685321783</v>
+      </c>
+      <c r="D13" t="n">
+        <v>18</v>
+      </c>
+      <c r="E13" t="n">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>jan/24</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>18622.48466946679</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8045804683335552</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>48750</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>fev/24</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>19234.56159767015</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.8132440322230873</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>52500</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>mar/24</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>17936.20928584332</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8127033877801724</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" t="n">
+        <v>52500</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>abr/24</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>16229.01935993407</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.8126781781720664</v>
+      </c>
+      <c r="D17" t="n">
         <v>4</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E17" t="n">
+        <v>56250</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>mai/24</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>13195.85421152111</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8118630875829163</v>
+      </c>
+      <c r="D18" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" t="n">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>jun/24</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>14213.88324067663</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.8029322487731854</v>
+      </c>
+      <c r="D19" t="n">
+        <v>8</v>
+      </c>
+      <c r="E19" t="n">
+        <v>63750</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>jul/24</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>13508.59077590868</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.79470936969161</v>
+      </c>
+      <c r="D20" t="n">
+        <v>8</v>
+      </c>
+      <c r="E20" t="n">
+        <v>67500</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>ago/24</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>11722.56196056255</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.7873186283509644</v>
+      </c>
+      <c r="D21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
+        <v>71250</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>set/24</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>17267.18009950432</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.7880267420062678</v>
+      </c>
+      <c r="D22" t="n">
         <v>13</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>15259.87</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.792</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="E22" t="n">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>out/24</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>12117.72764317709</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.7884565021202333</v>
+      </c>
+      <c r="D23" t="n">
+        <v>14</v>
+      </c>
+      <c r="E23" t="n">
+        <v>78750</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>nov/24</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>16782.89666367289</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.7886990707811938</v>
+      </c>
+      <c r="D24" t="n">
+        <v>16</v>
+      </c>
+      <c r="E24" t="n">
+        <v>82500</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>dez/24</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>20666.45292072826</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.794283904511367</v>
+      </c>
+      <c r="D25" t="n">
+        <v>17</v>
+      </c>
+      <c r="E25" t="n">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>jan/25</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>18546.87648412643</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.799595541300565</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>93750</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>fev/25</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>19560.64845962425</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.8047130849693235</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="n">
+        <v>97500</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>mar/25</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>15311.24572918876</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.8043914004280733</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>97500</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>abr/25</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>17293.25850103053</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.8045078371395596</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3</v>
+      </c>
+      <c r="E29" t="n">
+        <v>101250</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>mai/25</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>15944.8325643459</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.8043132843372615</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3</v>
+      </c>
+      <c r="E30" t="n">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>jun/25</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>13310.86694294293</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.7992819382473427</v>
+      </c>
+      <c r="D31" t="n">
+        <v>4</v>
+      </c>
+      <c r="E31" t="n">
+        <v>108750</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>jul/25</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>14014.89423378521</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.7946499976587363</v>
+      </c>
+      <c r="D32" t="n">
+        <v>5</v>
+      </c>
+      <c r="E32" t="n">
+        <v>112500</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>ago/25</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>14509.25156116502</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.7902610615639486</v>
+      </c>
+      <c r="D33" t="n">
         <v>6</v>
       </c>
-      <c r="D3" t="n">
-        <v>16</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>14690.19</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.794</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="E33" t="n">
+        <v>116250</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>set/25</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>14122.3579024505</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.7903084473061998</v>
+      </c>
+      <c r="D34" t="n">
+        <v>7</v>
+      </c>
+      <c r="E34" t="n">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>out/25</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>17288.54565333482</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.7904558062403007</v>
+      </c>
+      <c r="D35" t="n">
         <v>8</v>
       </c>
-      <c r="D4" t="n">
-        <v>28</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>15058.89</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.792</v>
-      </c>
-      <c r="C5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>26</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>15503.43</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.793</v>
-      </c>
-      <c r="C6" t="n">
-        <v>7</v>
-      </c>
-      <c r="D6" t="n">
-        <v>18</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>15621.04</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.794</v>
-      </c>
-      <c r="C7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="E35" t="n">
+        <v>123750</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>nov/25</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>16689.33753709613</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.7909278829800862</v>
+      </c>
+      <c r="D36" t="n">
+        <v>8</v>
+      </c>
+      <c r="E36" t="n">
+        <v>127500</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>dez/25</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>13969.81793243976</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.7947441667351274</v>
+      </c>
+      <c r="D37" t="n">
+        <v>10</v>
+      </c>
+      <c r="E37" t="n">
+        <v>135000</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>jan/26</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>17780.61194769814</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.798298703648135</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>138750</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>fev/26</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>15873.28124394189</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.801844332563743</v>
+      </c>
+      <c r="D39" t="n">
+        <v>3</v>
+      </c>
+      <c r="E39" t="n">
+        <v>142500</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>mar/26</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>16416.58613135264</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.8021261197863748</v>
+      </c>
+      <c r="D40" t="n">
+        <v>6</v>
+      </c>
+      <c r="E40" t="n">
+        <v>142500</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>abr/26</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>16352.82052936251</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.8021802743593284</v>
+      </c>
+      <c r="D41" t="n">
+        <v>8</v>
+      </c>
+      <c r="E41" t="n">
+        <v>146250</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>mai/26</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>16718.3236271229</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.802148840676981</v>
+      </c>
+      <c r="D42" t="n">
+        <v>9</v>
+      </c>
+      <c r="E42" t="n">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>jun/26</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>12525.91865312037</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.7986941201803853</v>
+      </c>
+      <c r="D43" t="n">
+        <v>9</v>
+      </c>
+      <c r="E43" t="n">
+        <v>153750</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>jul/26</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>10081.85840532218</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.7952398211072025</v>
+      </c>
+      <c r="D44" t="n">
+        <v>11</v>
+      </c>
+      <c r="E44" t="n">
+        <v>157500</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>ago/26</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>13428.30421469974</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.7921982014057595</v>
+      </c>
+      <c r="D45" t="n">
+        <v>11</v>
+      </c>
+      <c r="E45" t="n">
+        <v>161250</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>set/26</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>16448.63765055802</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.7924304342717142</v>
+      </c>
+      <c r="D46" t="n">
+        <v>12</v>
+      </c>
+      <c r="E46" t="n">
+        <v>165000</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>out/26</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>16876.32194335619</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.7925117235837611</v>
+      </c>
+      <c r="D47" t="n">
+        <v>13</v>
+      </c>
+      <c r="E47" t="n">
+        <v>168750</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>nov/26</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>16474.29318254084</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.7925271714383207</v>
+      </c>
+      <c r="D48" t="n">
         <v>14</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>14661.58</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.793</v>
-      </c>
-      <c r="C8" t="n">
-        <v>7</v>
-      </c>
-      <c r="D8" t="n">
-        <v>18</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>15434.04</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.796</v>
-      </c>
-      <c r="C9" t="n">
-        <v>5</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="E48" t="n">
+        <v>172500</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>dez/26</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>20115.47387448361</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.7952630890640563</v>
+      </c>
+      <c r="D49" t="n">
         <v>15</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>45000</v>
+      <c r="E49" t="n">
+        <v>180000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização final, nomeação do codigo
</commit_message>
<xml_diff>
--- a/tabela_energia_solar.xlsx
+++ b/tabela_energia_solar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,16 +467,18 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14018.03507989479</v>
+        <v>18281.41718200416</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9235312949144248</v>
+        <v>0.9253470427691208</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" t="n">
-        <v>3750</v>
+        <v>2</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>3750.0</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -486,16 +488,18 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14949.49595783571</v>
+        <v>16988.40299142623</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9246679758811538</v>
+        <v>0.9237431992000914</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E3" t="n">
-        <v>7500</v>
+        <v>4</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>7500.0</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -505,16 +509,18 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>14537.74260832353</v>
+        <v>15138.62007278379</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8824736461578573</v>
+        <v>0.8822813921639386</v>
       </c>
       <c r="D4" t="n">
         <v>7</v>
       </c>
-      <c r="E4" t="n">
-        <v>7500</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>7500.0</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -524,16 +530,18 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>18279.91016327494</v>
+        <v>15329.35884692755</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8613172748742098</v>
+        <v>0.8635122460689554</v>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" t="n">
-        <v>11250</v>
+        <v>8</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>11250.0</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -543,16 +551,18 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>16255.19719269662</v>
+        <v>15688.72761361258</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8502538146157599</v>
+        <v>0.8502895741668449</v>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" t="n">
-        <v>15000</v>
+        <v>9</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>15000.0</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -562,16 +572,18 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>13805.29103056303</v>
+        <v>12831.01436390388</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8168052326229519</v>
+        <v>0.817068167631756</v>
       </c>
       <c r="D7" t="n">
-        <v>11</v>
-      </c>
-      <c r="E7" t="n">
-        <v>18750</v>
+        <v>10</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>18750.0</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -581,16 +593,18 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>13941.99561851709</v>
+        <v>11032.65748020475</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7929034671484142</v>
+        <v>0.7925967034287786</v>
       </c>
       <c r="D8" t="n">
-        <v>11</v>
-      </c>
-      <c r="E8" t="n">
-        <v>22500</v>
+        <v>13</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>22500.0</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -600,16 +614,18 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>15474.86621416792</v>
+        <v>13727.04797101636</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7756964490890278</v>
+        <v>0.774338392234531</v>
       </c>
       <c r="D9" t="n">
-        <v>12</v>
-      </c>
-      <c r="E9" t="n">
-        <v>26250</v>
+        <v>14</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>26250.0</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -619,16 +635,18 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>14726.45210408088</v>
+        <v>16891.61084189163</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7787962977969178</v>
+        <v>0.7765295046034784</v>
       </c>
       <c r="D10" t="n">
-        <v>14</v>
-      </c>
-      <c r="E10" t="n">
-        <v>30000</v>
+        <v>15</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>R$ 30000.0</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -638,16 +656,18 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>15528.80960014159</v>
+        <v>14491.24595901378</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7810320899749387</v>
+        <v>0.7788893252838881</v>
       </c>
       <c r="D11" t="n">
-        <v>14</v>
-      </c>
-      <c r="E11" t="n">
-        <v>33750</v>
+        <v>16</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>R$ 33750.0</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -657,16 +677,18 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>15414.1665471413</v>
+        <v>14837.22323708005</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7827224030655975</v>
+        <v>0.7806320160734787</v>
       </c>
       <c r="D12" t="n">
-        <v>17</v>
-      </c>
-      <c r="E12" t="n">
-        <v>37500</v>
+        <v>16</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>R$ 37500.0</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -676,16 +698,18 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>20772.72079654977</v>
+        <v>17394.85150841544</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7947069685321783</v>
+        <v>0.7927217252827734</v>
       </c>
       <c r="D13" t="n">
         <v>18</v>
       </c>
-      <c r="E13" t="n">
-        <v>45000</v>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>45000.0</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -695,16 +719,18 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>18622.48466946679</v>
+        <v>17416.93717556038</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8045804683335552</v>
+        <v>0.8031720224839115</v>
       </c>
       <c r="D14" t="n">
         <v>1</v>
       </c>
-      <c r="E14" t="n">
-        <v>48750</v>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>48750.0</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -714,16 +740,18 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>19234.56159767015</v>
+        <v>15790.867952961</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8132440322230873</v>
+        <v>0.8122238662582639</v>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" t="n">
-        <v>52500</v>
+        <v>4</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>52500.0</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -733,16 +761,18 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>17936.20928584332</v>
+        <v>14839.59745432269</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8127033877801724</v>
+        <v>0.811194898644345</v>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
-      </c>
-      <c r="E16" t="n">
-        <v>52500</v>
+        <v>6</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>52500.0</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -752,16 +782,18 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>16229.01935993407</v>
+        <v>13749.78632276983</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8126781781720664</v>
+        <v>0.8102806569385593</v>
       </c>
       <c r="D17" t="n">
-        <v>4</v>
-      </c>
-      <c r="E17" t="n">
-        <v>56250</v>
+        <v>6</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>56250.0</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -771,16 +803,18 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>13195.85421152111</v>
+        <v>15333.23503372919</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8118630875829163</v>
+        <v>0.810104974446743</v>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
-      </c>
-      <c r="E18" t="n">
-        <v>60000</v>
+        <v>7</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>60000.0</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -790,16 +824,18 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>14213.88324067663</v>
+        <v>11467.56037527807</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8029322487731854</v>
+        <v>0.8014208663518329</v>
       </c>
       <c r="D19" t="n">
-        <v>8</v>
-      </c>
-      <c r="E19" t="n">
-        <v>63750</v>
+        <v>10</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>63750.0</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -809,16 +845,18 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>13508.59077590868</v>
+        <v>13395.57447862929</v>
       </c>
       <c r="C20" t="n">
-        <v>0.79470936969161</v>
+        <v>0.7933730752686512</v>
       </c>
       <c r="D20" t="n">
-        <v>8</v>
-      </c>
-      <c r="E20" t="n">
-        <v>67500</v>
+        <v>11</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>67500.0</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -828,16 +866,18 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>11722.56196056255</v>
+        <v>11571.09963335015</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7873186283509644</v>
+        <v>0.7864564168385478</v>
       </c>
       <c r="D21" t="n">
-        <v>10</v>
-      </c>
-      <c r="E21" t="n">
-        <v>71250</v>
+        <v>12</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>71250.0</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -847,16 +887,18 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17267.18009950432</v>
+        <v>17037.44766788312</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7880267420062678</v>
+        <v>0.787430307481391</v>
       </c>
       <c r="D22" t="n">
-        <v>13</v>
-      </c>
-      <c r="E22" t="n">
-        <v>75000</v>
+        <v>12</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>R$ 75000.0</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -866,16 +908,18 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>12117.72764317709</v>
+        <v>15095.80317128141</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7884565021202333</v>
+        <v>0.7883326271148985</v>
       </c>
       <c r="D23" t="n">
-        <v>14</v>
-      </c>
-      <c r="E23" t="n">
-        <v>78750</v>
+        <v>15</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>R$ 78750.0</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -885,16 +929,18 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>16782.89666367289</v>
+        <v>13509.88755883382</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7886990707811938</v>
+        <v>0.7889865652206417</v>
       </c>
       <c r="D24" t="n">
-        <v>16</v>
-      </c>
-      <c r="E24" t="n">
-        <v>82500</v>
+        <v>18</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>R$ 82500.0</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -904,16 +950,18 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>20666.45292072826</v>
+        <v>20758.60800665064</v>
       </c>
       <c r="C25" t="n">
-        <v>0.794283904511367</v>
+        <v>0.794777321188505</v>
       </c>
       <c r="D25" t="n">
-        <v>17</v>
-      </c>
-      <c r="E25" t="n">
-        <v>90000</v>
+        <v>19</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>90000.0</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -923,16 +971,18 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>18546.87648412643</v>
+        <v>19564.75581795489</v>
       </c>
       <c r="C26" t="n">
-        <v>0.799595541300565</v>
+        <v>0.7999825175485745</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" t="n">
-        <v>93750</v>
+        <v>3</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>93750.0</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -942,16 +992,18 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>19560.64845962425</v>
+        <v>19599.33063688026</v>
       </c>
       <c r="C27" t="n">
-        <v>0.8047130849693235</v>
+        <v>0.8047900336335853</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" t="n">
-        <v>97500</v>
+        <v>4</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>97500.0</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -961,16 +1013,18 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>15311.24572918876</v>
+        <v>15448.54831319266</v>
       </c>
       <c r="C28" t="n">
-        <v>0.8043914004280733</v>
+        <v>0.8048763811098819</v>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
-      </c>
-      <c r="E28" t="n">
-        <v>97500</v>
+        <v>5</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>97500.0</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -980,16 +1034,18 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>17293.25850103053</v>
+        <v>16436.97412688972</v>
       </c>
       <c r="C29" t="n">
-        <v>0.8045078371395596</v>
+        <v>0.8044648373404816</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
-      </c>
-      <c r="E29" t="n">
-        <v>101250</v>
+        <v>7</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>101250.0</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -999,16 +1055,18 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>15944.8325643459</v>
+        <v>15331.56081419541</v>
       </c>
       <c r="C30" t="n">
-        <v>0.8043132843372615</v>
+        <v>0.804423480645267</v>
       </c>
       <c r="D30" t="n">
-        <v>3</v>
-      </c>
-      <c r="E30" t="n">
-        <v>105000</v>
+        <v>9</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>105000.0</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1018,16 +1076,18 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>13310.86694294293</v>
+        <v>12340.03562991894</v>
       </c>
       <c r="C31" t="n">
-        <v>0.7992819382473427</v>
+        <v>0.7993561688978712</v>
       </c>
       <c r="D31" t="n">
-        <v>4</v>
-      </c>
-      <c r="E31" t="n">
-        <v>108750</v>
+        <v>13</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>108750.0</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -1037,16 +1097,18 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>14014.89423378521</v>
+        <v>12168.44152189638</v>
       </c>
       <c r="C32" t="n">
-        <v>0.7946499976587363</v>
+        <v>0.7947819179257937</v>
       </c>
       <c r="D32" t="n">
-        <v>5</v>
-      </c>
-      <c r="E32" t="n">
-        <v>112500</v>
+        <v>15</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>112500.0</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -1056,16 +1118,18 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>14509.25156116502</v>
+        <v>14037.74855524926</v>
       </c>
       <c r="C33" t="n">
-        <v>0.7902610615639486</v>
+        <v>0.790050084011784</v>
       </c>
       <c r="D33" t="n">
-        <v>6</v>
-      </c>
-      <c r="E33" t="n">
-        <v>116250</v>
+        <v>15</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>116250.0</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -1075,16 +1139,18 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>14122.3579024505</v>
+        <v>17075.36618346194</v>
       </c>
       <c r="C34" t="n">
-        <v>0.7903084473061998</v>
+        <v>0.7900600783645892</v>
       </c>
       <c r="D34" t="n">
-        <v>7</v>
-      </c>
-      <c r="E34" t="n">
-        <v>120000</v>
+        <v>16</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>R$ 120000.0</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -1094,16 +1160,18 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17288.54565333482</v>
+        <v>18327.05105936733</v>
       </c>
       <c r="C35" t="n">
-        <v>0.7904558062403007</v>
+        <v>0.7901683527887144</v>
       </c>
       <c r="D35" t="n">
-        <v>8</v>
-      </c>
-      <c r="E35" t="n">
-        <v>123750</v>
+        <v>17</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>R$ 123750.0</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1113,16 +1181,18 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>16689.33753709613</v>
+        <v>17374.93798230206</v>
       </c>
       <c r="C36" t="n">
-        <v>0.7909278829800862</v>
+        <v>0.7905743191398917</v>
       </c>
       <c r="D36" t="n">
-        <v>8</v>
-      </c>
-      <c r="E36" t="n">
-        <v>127500</v>
+        <v>17</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>R$ 127500.0</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -1132,16 +1202,18 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>13969.81793243976</v>
+        <v>17910.38833912814</v>
       </c>
       <c r="C37" t="n">
-        <v>0.7947441667351274</v>
+        <v>0.7943084354472331</v>
       </c>
       <c r="D37" t="n">
-        <v>10</v>
-      </c>
-      <c r="E37" t="n">
-        <v>135000</v>
+        <v>17</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>135000.0</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -1151,16 +1223,18 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>17780.61194769814</v>
+        <v>17575.95149213711</v>
       </c>
       <c r="C38" t="n">
-        <v>0.798298703648135</v>
+        <v>0.7978825349736277</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" t="n">
-        <v>138750</v>
+        <v>2</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>138750.0</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -1170,16 +1244,18 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>15873.28124394189</v>
+        <v>20758.92107516381</v>
       </c>
       <c r="C39" t="n">
-        <v>0.801844332563743</v>
+        <v>0.8012510092141002</v>
       </c>
       <c r="D39" t="n">
-        <v>3</v>
-      </c>
-      <c r="E39" t="n">
-        <v>142500</v>
+        <v>2</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>142500.0</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -1189,16 +1265,18 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>16416.58613135264</v>
+        <v>14608.62739231304</v>
       </c>
       <c r="C40" t="n">
-        <v>0.8021261197863748</v>
+        <v>0.8011297725113408</v>
       </c>
       <c r="D40" t="n">
-        <v>6</v>
-      </c>
-      <c r="E40" t="n">
-        <v>142500</v>
+        <v>2</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>142500.0</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -1208,16 +1286,18 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>16352.82052936251</v>
+        <v>15750.02792188644</v>
       </c>
       <c r="C41" t="n">
-        <v>0.8021802743593284</v>
+        <v>0.8008585967290578</v>
       </c>
       <c r="D41" t="n">
-        <v>8</v>
-      </c>
-      <c r="E41" t="n">
-        <v>146250</v>
+        <v>4</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>146250.0</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -1227,16 +1307,18 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>16718.3236271229</v>
+        <v>18327.21933741934</v>
       </c>
       <c r="C42" t="n">
-        <v>0.802148840676981</v>
+        <v>0.8008664952022444</v>
       </c>
       <c r="D42" t="n">
-        <v>9</v>
-      </c>
-      <c r="E42" t="n">
-        <v>150000</v>
+        <v>5</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>150000.0</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -1246,16 +1328,18 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>12525.91865312037</v>
+        <v>14279.56204967202</v>
       </c>
       <c r="C43" t="n">
-        <v>0.7986941201803853</v>
+        <v>0.7973087841620411</v>
       </c>
       <c r="D43" t="n">
-        <v>9</v>
-      </c>
-      <c r="E43" t="n">
-        <v>153750</v>
+        <v>5</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>153750.0</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -1265,16 +1349,18 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>10081.85840532218</v>
+        <v>11700.16644399979</v>
       </c>
       <c r="C44" t="n">
-        <v>0.7952398211072025</v>
+        <v>0.7940419144975744</v>
       </c>
       <c r="D44" t="n">
-        <v>11</v>
-      </c>
-      <c r="E44" t="n">
-        <v>157500</v>
+        <v>7</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>157500.0</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -1284,16 +1370,18 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>13428.30421469974</v>
+        <v>10910.8910444108</v>
       </c>
       <c r="C45" t="n">
-        <v>0.7921982014057595</v>
+        <v>0.7909338069727823</v>
       </c>
       <c r="D45" t="n">
-        <v>11</v>
-      </c>
-      <c r="E45" t="n">
-        <v>161250</v>
+        <v>10</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>161250.0</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -1303,16 +1391,18 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>16448.63765055802</v>
+        <v>18157.71134994925</v>
       </c>
       <c r="C46" t="n">
-        <v>0.7924304342717142</v>
+        <v>0.7911537851723541</v>
       </c>
       <c r="D46" t="n">
-        <v>12</v>
-      </c>
-      <c r="E46" t="n">
-        <v>165000</v>
+        <v>10</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>R$ 165000.0</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -1322,16 +1412,18 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>16876.32194335619</v>
+        <v>16964.74151877666</v>
       </c>
       <c r="C47" t="n">
-        <v>0.7925117235837611</v>
+        <v>0.7914634370895023</v>
       </c>
       <c r="D47" t="n">
-        <v>13</v>
-      </c>
-      <c r="E47" t="n">
-        <v>168750</v>
+        <v>12</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>R$ 168750.0</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -1341,16 +1433,18 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>16474.29318254084</v>
+        <v>14066.77393230765</v>
       </c>
       <c r="C48" t="n">
-        <v>0.7925271714383207</v>
+        <v>0.7915948282657317</v>
       </c>
       <c r="D48" t="n">
-        <v>14</v>
-      </c>
-      <c r="E48" t="n">
-        <v>172500</v>
+        <v>15</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>R$ 172500.0</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -1360,16 +1454,1026 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>20115.47387448361</v>
+        <v>17313.41004505829</v>
       </c>
       <c r="C49" t="n">
-        <v>0.7952630890640563</v>
+        <v>0.7942949419759341</v>
       </c>
       <c r="D49" t="n">
+        <v>16</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>180000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>jan/23</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>16645.30719604437</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.9216666396555492</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>3750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>fev/23</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>16974.63542286582</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.9226424589108764</v>
+      </c>
+      <c r="D51" t="n">
+        <v>3</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>7500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>mar/23</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>14425.14961577128</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.8840448538020353</v>
+      </c>
+      <c r="D52" t="n">
+        <v>5</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>7500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>abr/23</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>17671.52255239887</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.8642621199097834</v>
+      </c>
+      <c r="D53" t="n">
+        <v>6</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>11250.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>mai/23</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>15808.49483473181</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.8529691087488216</v>
+      </c>
+      <c r="D54" t="n">
+        <v>7</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>15000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>jun/23</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>13034.0023261628</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.8184461582976881</v>
+      </c>
+      <c r="D55" t="n">
+        <v>8</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>18750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>jul/23</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>12944.85076067505</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.7951706701505089</v>
+      </c>
+      <c r="D56" t="n">
+        <v>11</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>22500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>ago/23</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>12475.19475358986</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.7772482150442607</v>
+      </c>
+      <c r="D57" t="n">
+        <v>14</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>26250.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>set/23</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>15645.39553422554</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.7802915624447082</v>
+      </c>
+      <c r="D58" t="n">
+        <v>17</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>R$ 30000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>out/23</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>16867.97588210376</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.7827554560761584</v>
+      </c>
+      <c r="D59" t="n">
+        <v>18</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>R$ 33750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>nov/23</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>15922.19455516386</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.7841716684991714</v>
+      </c>
+      <c r="D60" t="n">
+        <v>19</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>R$ 37500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>dez/23</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>17038.48531095783</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.7960634271780483</v>
+      </c>
+      <c r="D61" t="n">
+        <v>21</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>45000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>jan/24</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>19228.53916324906</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.805916612594364</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>48750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>fev/24</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>19625.01626468029</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.8144017851426968</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>52500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>mar/24</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>15614.60476633806</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.8132661399652499</v>
+      </c>
+      <c r="D64" t="n">
+        <v>2</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>52500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>abr/24</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>17660.2791797764</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.8129121493016128</v>
+      </c>
+      <c r="D65" t="n">
+        <v>2</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>56250.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>mai/24</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>14508.22474384626</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.8126550674857184</v>
+      </c>
+      <c r="D66" t="n">
+        <v>7</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>60000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>jun/24</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>11706.40155197544</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.8034215255042887</v>
+      </c>
+      <c r="D67" t="n">
+        <v>7</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>63750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>jul/24</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>13343.97817446976</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.7949876188428766</v>
+      </c>
+      <c r="D68" t="n">
+        <v>8</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>67500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>ago/24</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>12121.31273014654</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.7879454012516042</v>
+      </c>
+      <c r="D69" t="n">
+        <v>10</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>71250.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>set/24</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>15526.89043111635</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.7887036518388165</v>
+      </c>
+      <c r="D70" t="n">
+        <v>14</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>R$ 75000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>out/24</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>16299.63523987762</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.7894297551735668</v>
+      </c>
+      <c r="D71" t="n">
         <v>15</v>
       </c>
-      <c r="E49" t="n">
-        <v>180000</v>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>R$ 78750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>nov/24</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>15030.77078971413</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.7898599346125853</v>
+      </c>
+      <c r="D72" t="n">
+        <v>16</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>R$ 82500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>dez/24</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>21846.87476889419</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.7955787999702389</v>
+      </c>
+      <c r="D73" t="n">
+        <v>16</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>90000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>jan/25</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>18031.98184953722</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.800530021054854</v>
+      </c>
+      <c r="D74" t="n">
+        <v>2</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>93750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>fev/25</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>16172.64393118808</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.8054580995222469</v>
+      </c>
+      <c r="D75" t="n">
+        <v>2</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>97500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>mar/25</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>15559.88269570157</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.8052091355139847</v>
+      </c>
+      <c r="D76" t="n">
+        <v>3</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>97500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>abr/25</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>14033.63883253741</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.8048556628238039</v>
+      </c>
+      <c r="D77" t="n">
+        <v>4</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>101250.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>mai/25</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>16524.95989701298</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.8046726328873065</v>
+      </c>
+      <c r="D78" t="n">
+        <v>5</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>105000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>jun/25</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>11896.31359824639</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.7998838671799858</v>
+      </c>
+      <c r="D79" t="n">
+        <v>9</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>108750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>jul/25</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>14474.62855338611</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.7951356801816843</v>
+      </c>
+      <c r="D80" t="n">
+        <v>9</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>112500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>ago/25</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>13081.22776607373</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.7906811992436015</v>
+      </c>
+      <c r="D81" t="n">
+        <v>12</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>116250.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>set/25</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>14793.93099452905</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.791003967825978</v>
+      </c>
+      <c r="D82" t="n">
+        <v>13</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>R$ 120000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>out/25</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>13020.67039188909</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.790910191533391</v>
+      </c>
+      <c r="D83" t="n">
+        <v>14</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>R$ 123750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>nov/25</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>15930.18109553455</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.7909565375412809</v>
+      </c>
+      <c r="D84" t="n">
+        <v>15</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>R$ 127500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>dez/25</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>17848.50290165483</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.794806582485524</v>
+      </c>
+      <c r="D85" t="n">
+        <v>16</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>135000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>jan/26</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>20270.52042194463</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.7982847736921228</v>
+      </c>
+      <c r="D86" t="n">
+        <v>1</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>138750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>fev/26</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>19588.40130635247</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.8016056775083776</v>
+      </c>
+      <c r="D87" t="n">
+        <v>1</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>142500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>mar/26</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>15771.12733540935</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.8016045989104308</v>
+      </c>
+      <c r="D88" t="n">
+        <v>3</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>142500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>abr/26</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>17759.66115185539</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.8017344263554252</v>
+      </c>
+      <c r="D89" t="n">
+        <v>4</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>146250.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>mai/26</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>16262.41772182831</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.8017060493838002</v>
+      </c>
+      <c r="D90" t="n">
+        <v>6</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>150000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>jun/26</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>12199.39589084536</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.7980799794567823</v>
+      </c>
+      <c r="D91" t="n">
+        <v>9</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>153750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>jul/26</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>13493.64284124676</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.7947029479484123</v>
+      </c>
+      <c r="D92" t="n">
+        <v>11</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>157500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>ago/26</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>13477.05435448658</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.7914969790313241</v>
+      </c>
+      <c r="D93" t="n">
+        <v>12</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>161250.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>set/26</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>14147.83868296486</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.7917109498014188</v>
+      </c>
+      <c r="D94" t="n">
+        <v>15</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>R$ 165000.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>out/26</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>14956.24471101704</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.7919601326506848</v>
+      </c>
+      <c r="D95" t="n">
+        <v>20</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>R$ 168750.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>nov/26</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>15978.87116369352</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.7921297468224102</v>
+      </c>
+      <c r="D96" t="n">
+        <v>23</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>R$ 172500.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>dez/26</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>20537.21806523818</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0.7949109153177442</v>
+      </c>
+      <c r="D97" t="n">
+        <v>23</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>180000.0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>